<commit_message>
Updated pinout and BOM for PCB
</commit_message>
<xml_diff>
--- a/documentation/MegaPinout.xlsx
+++ b/documentation/MegaPinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Dropbox\Engineering\STEVE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\GitHub\steve\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="181">
   <si>
     <t>Pin Number</t>
   </si>
@@ -561,6 +561,12 @@
   </si>
   <si>
     <t>IN_4</t>
+  </si>
+  <si>
+    <t>BATTERY</t>
+  </si>
+  <si>
+    <t>V_batt</t>
   </si>
 </sst>
 </file>
@@ -924,8 +930,8 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +2005,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2020,8 +2026,14 @@
       <c r="C98" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>179</v>
+      </c>
+      <c r="E98" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2032,7 +2044,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2043,7 +2055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Updated electronics box, added grill, updated pinout, added code for power board
</commit_message>
<xml_diff>
--- a/documentation/MegaPinout.xlsx
+++ b/documentation/MegaPinout.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="184">
   <si>
     <t>Pin Number</t>
   </si>
@@ -567,6 +568,15 @@
   </si>
   <si>
     <t>V_batt</t>
+  </si>
+  <si>
+    <t>PWR BOARD</t>
+  </si>
+  <si>
+    <t>MOTOR_EN</t>
+  </si>
+  <si>
+    <t>PI_EN</t>
   </si>
 </sst>
 </file>
@@ -930,8 +940,8 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,6 +1546,12 @@
       <c r="C54" t="s">
         <v>89</v>
       </c>
+      <c r="D54" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -1546,6 +1562,12 @@
       </c>
       <c r="C55" t="s">
         <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>181</v>
+      </c>
+      <c r="E55" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>